<commit_message>
update the ui by py and the .exe file by cpp
</commit_message>
<xml_diff>
--- a/py/1data.xlsx
+++ b/py/1data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,25 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27945" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11580"/>
   </bookViews>
   <sheets>
-    <sheet name="Trading Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -37,36 +24,40 @@
     <t>Emotion Values</t>
   </si>
   <si>
-    <t>Position Ratio</t>
+    <t>Price Changes</t>
   </si>
   <si>
-    <t>Price Changes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Actual Capital</t>
   </si>
   <si>
     <t>Daily Return</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Actual Capital</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>0.43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -79,7 +70,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,16 +78,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,351 +404,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.75" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2">
         <v>17000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0.98</v>
-      </c>
-      <c r="C3" s="1">
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.98</v>
-      </c>
-      <c r="C4" s="1">
         <v>3.5299999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>0.63100000000000001</v>
       </c>
       <c r="B5">
-        <v>0.98</v>
-      </c>
-      <c r="C5" s="1">
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>0.71</v>
       </c>
       <c r="B6">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="C6" s="1">
         <v>5.4100000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>0.37</v>
       </c>
       <c r="B7">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="C7" s="1">
         <v>3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>0.54</v>
       </c>
       <c r="B8">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="C8" s="1">
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>0.44</v>
       </c>
       <c r="B9">
-        <f>16237/17273</f>
-        <v>0.94002199965263711</v>
-      </c>
-      <c r="C9" s="1">
         <v>2.53E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>0.6</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
         <v>4.3499999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>0.09</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.96</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11">
         <v>1.12E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>0.2</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B12">
         <v>2.6700000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>0.11</v>
       </c>
-      <c r="B13" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="C13" s="1">
-        <f>(D13-D2)/D2</f>
+      <c r="B13">
         <v>0.11</v>
       </c>
-      <c r="D13" s="3">
+      <c r="C13">
         <v>18870</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.98799999999999999</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D14" s="3">
+      <c r="C14">
         <v>19010</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>0.06</v>
       </c>
-      <c r="B15" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B15">
         <v>0.1095</v>
       </c>
-      <c r="D15" s="3">
+      <c r="C15">
         <v>18861</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>0.16</v>
       </c>
       <c r="B16">
-        <f>18207/19983</f>
-        <v>0.9111244557874193</v>
+        <v>0.17547058823529399</v>
       </c>
       <c r="C16">
-        <f>(19983-17000)/17000</f>
-        <v>0.17547058823529413</v>
-      </c>
-      <c r="D16" s="3">
         <v>19983</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>0.42</v>
       </c>
       <c r="B17">
-        <f>17586/D17</f>
-        <v>0.908227030935289</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="C17">
-        <f>(D17-D2)/D2</f>
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="D17" s="3">
         <v>19363</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>0.59</v>
       </c>
       <c r="B18">
-        <f>17937/D18</f>
-        <v>0.88841010401188703</v>
+        <v>0.187647058823529</v>
       </c>
       <c r="C18">
-        <f>(D18-D2)/D2</f>
-        <v>0.18764705882352942</v>
-      </c>
-      <c r="D18" s="3">
         <v>20190</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>0.1</v>
       </c>
       <c r="B19">
-        <f>18810/D19</f>
-        <v>0.94884987893462469</v>
+        <v>0.16611764705882401</v>
       </c>
       <c r="C19">
-        <f>(D19-D2)/D2</f>
-        <v>0.16611764705882354</v>
-      </c>
-      <c r="D19" s="3">
         <v>19824</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>0.13</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.17647058823529399</v>
       </c>
       <c r="C20">
-        <f>(D20-D2)/D2</f>
-        <v>0.17647058823529413</v>
-      </c>
-      <c r="D20" s="3">
         <v>20000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>0.16</v>
       </c>
       <c r="B21">
-        <f>19480/20134</f>
-        <v>0.96751763186649453</v>
+        <v>0.184352941176471</v>
       </c>
       <c r="C21">
-        <f>(20134-17000)/17000</f>
-        <v>0.18435294117647058</v>
-      </c>
-      <c r="D21" s="3">
         <v>20134</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>0.25</v>
       </c>
       <c r="B22">
-        <f>19550/20205</f>
-        <v>0.96758228161346205</v>
+        <v>0.188529411764706</v>
       </c>
       <c r="C22">
-        <f>(20205-17000)/17000</f>
-        <v>0.18852941176470589</v>
-      </c>
-      <c r="D22" s="3">
         <v>20205</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>0.19</v>
       </c>
       <c r="B23">
-        <f>18320/18975</f>
-        <v>0.96548089591567854</v>
+        <v>0.11617647058823501</v>
       </c>
       <c r="C23">
-        <f>(18975-17000)/17000</f>
-        <v>0.1161764705882353</v>
-      </c>
-      <c r="D23" s="3">
         <v>18975</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>0.31</v>
       </c>
       <c r="B24">
-        <f>18390/19045</f>
-        <v>0.96560777106852191</v>
+        <v>0.120294117647059</v>
       </c>
       <c r="C24">
-        <f>(19045-17000)/17000</f>
-        <v>0.12029411764705883</v>
-      </c>
-      <c r="D24" s="3">
         <v>19045</v>
       </c>
-      <c r="E24">
+      <c r="D24">
         <v>0.37</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C25">
+        <v>18286</v>
+      </c>
+      <c r="D25">
+        <v>-3.88</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add transformer train set and model
</commit_message>
<xml_diff>
--- a/py/1data.xlsx
+++ b/py/1data.xlsx
@@ -1,70 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EmotionCat\py\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11580"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Emotion Values</t>
-  </si>
-  <si>
-    <t>Price Changes</t>
-  </si>
-  <si>
-    <t>Actual Capital</t>
-  </si>
-  <si>
-    <t>Daily Return</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -79,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -403,269 +420,342 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Emotion Values</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Price Changes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Actual Capital</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Daily Return</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>17000</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="B3" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>7.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>3.5299999999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>0.63100000000000001</v>
-      </c>
-      <c r="B5">
-        <v>9.9000000000000008E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="B4" t="n">
+        <v>0.0353</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.631</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.009900000000000001</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>0.71</v>
       </c>
-      <c r="B6">
-        <v>5.4100000000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="B6" t="n">
+        <v>0.0541</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>0.37</v>
       </c>
-      <c r="B7">
-        <v>3.6799999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="B7" t="n">
+        <v>0.0368</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>0.54</v>
       </c>
-      <c r="B8">
-        <v>4.4200000000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="B8" t="n">
+        <v>0.0442</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>0.44</v>
       </c>
-      <c r="B9">
-        <v>2.53E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="B9" t="n">
+        <v>0.0253</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>0.6</v>
       </c>
-      <c r="B10">
-        <v>4.3499999999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="B10" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>0.09</v>
       </c>
-      <c r="B11">
-        <v>1.12E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="B11" t="n">
+        <v>0.0112</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>0.2</v>
       </c>
-      <c r="B12">
-        <v>2.6700000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="B12" t="n">
+        <v>0.0267</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>0.11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>0.11</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>18870</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="B14">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="C14">
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.118</v>
+      </c>
+      <c r="C14" t="n">
         <v>19010</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>0.06</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>0.1095</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>18861</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>0.16</v>
       </c>
-      <c r="B16">
-        <v>0.17547058823529399</v>
-      </c>
-      <c r="C16">
+      <c r="B16" t="n">
+        <v>0.175470588235294</v>
+      </c>
+      <c r="C16" t="n">
         <v>19983</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="D16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>0.42</v>
       </c>
-      <c r="B17">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="C17">
+      <c r="B17" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="C17" t="n">
         <v>19363</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="D17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>0.59</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>0.187647058823529</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>20190</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="D18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>0.1</v>
       </c>
-      <c r="B19">
-        <v>0.16611764705882401</v>
-      </c>
-      <c r="C19">
+      <c r="B19" t="n">
+        <v>0.166117647058824</v>
+      </c>
+      <c r="C19" t="n">
         <v>19824</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="D19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>0.13</v>
       </c>
-      <c r="B20">
-        <v>0.17647058823529399</v>
-      </c>
-      <c r="C20">
+      <c r="B20" t="n">
+        <v>0.176470588235294</v>
+      </c>
+      <c r="C20" t="n">
         <v>20000</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="D20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>0.16</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>0.184352941176471</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>20134</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="D21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>0.25</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>0.188529411764706</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>20205</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="D22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
         <v>0.19</v>
       </c>
-      <c r="B23">
-        <v>0.11617647058823501</v>
-      </c>
-      <c r="C23">
+      <c r="B23" t="n">
+        <v>0.116176470588235</v>
+      </c>
+      <c r="C23" t="n">
         <v>18975</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="D23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
         <v>0.31</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>0.120294117647059</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>19045</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>0.37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="C25">
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="C25" t="n">
         <v>18286</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>-3.88</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="C26" t="n">
+        <v>18479</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="C27" t="n">
+        <v>18591</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.61</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update the source code
</commit_message>
<xml_diff>
--- a/py/1data.xlsx
+++ b/py/1data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,10 +740,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
+      <c r="A27" t="n">
+        <v>0.01</v>
       </c>
       <c r="B27" t="n">
         <v>0.094</v>
@@ -753,6 +751,36 @@
       </c>
       <c r="D27" t="n">
         <v>0.61</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="C28" t="n">
+        <v>18431</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.86</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="C29" t="n">
+        <v>17528</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-4.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>